<commit_message>
last data entry before leaving la selva
</commit_message>
<xml_diff>
--- a/raw_data/fern_dryweights.csv.xlsx
+++ b/raw_data/fern_dryweights.csv.xlsx
@@ -13,15 +13,13 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="560" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="562" uniqueCount="67">
   <si>
     <t>site</t>
   </si>
@@ -216,13 +214,19 @@
   </si>
   <si>
     <t>na</t>
+  </si>
+  <si>
+    <t>2a</t>
+  </si>
+  <si>
+    <t>2b</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -233,6 +237,12 @@
     <font>
       <sz val="10"/>
       <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -257,7 +267,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -271,6 +281,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -610,17 +623,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J156"/>
+  <dimension ref="A1:L156"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+      <pane ySplit="1" topLeftCell="A149" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I161" sqref="I161"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="9.140625" style="3"/>
-    <col min="3" max="3" width="23.140625" style="3" customWidth="1"/>
-    <col min="4" max="7" width="9.140625" style="3"/>
+    <col min="3" max="3" width="27.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="9.140625" style="3"/>
     <col min="8" max="8" width="12.28515625" style="3" customWidth="1"/>
     <col min="9" max="9" width="12.7109375" style="3" customWidth="1"/>
     <col min="10" max="10" width="9.140625" style="3"/>
@@ -991,10 +1006,10 @@
         <v>1.4E-3</v>
       </c>
       <c r="H13" s="5">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I13" s="5">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1020,10 +1035,10 @@
         <v>8.0000000000000004E-4</v>
       </c>
       <c r="H14" s="5">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I14" s="5">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1049,10 +1064,10 @@
         <v>1.1999999999999999E-3</v>
       </c>
       <c r="H15" s="5">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I15" s="5">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1078,10 +1093,10 @@
         <v>5.9999999999999995E-4</v>
       </c>
       <c r="H16" s="5">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="I16" s="5">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1107,10 +1122,10 @@
         <v>1.6000000000000001E-3</v>
       </c>
       <c r="H17" s="5">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="I17" s="5">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1136,10 +1151,10 @@
         <v>1.1000000000000001E-3</v>
       </c>
       <c r="H18" s="5">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I18" s="5">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1165,10 +1180,10 @@
         <v>5.4999999999999997E-3</v>
       </c>
       <c r="H19" s="5">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I19" s="5">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1192,10 +1207,10 @@
       </c>
       <c r="G20" s="5"/>
       <c r="H20" s="5">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I20" s="5">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1221,10 +1236,10 @@
         <v>6.4999999999999997E-3</v>
       </c>
       <c r="H21" s="5">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I21" s="5">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1250,10 +1265,10 @@
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="H22" s="5">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I22" s="5">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1279,10 +1294,10 @@
         <v>5.3E-3</v>
       </c>
       <c r="H23" s="5">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I23" s="5">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1308,10 +1323,10 @@
         <v>6.0000000000000001E-3</v>
       </c>
       <c r="H24" s="5">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I24" s="5">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1337,10 +1352,10 @@
         <v>5.3E-3</v>
       </c>
       <c r="H25" s="5">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I25" s="5">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1366,10 +1381,10 @@
         <v>4.4000000000000003E-3</v>
       </c>
       <c r="H26" s="5">
+        <v>10</v>
+      </c>
+      <c r="I26" s="5">
         <v>2</v>
-      </c>
-      <c r="I26" s="5">
-        <v>10</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1395,10 +1410,10 @@
         <v>4.3E-3</v>
       </c>
       <c r="H27" s="5">
+        <v>10</v>
+      </c>
+      <c r="I27" s="5">
         <v>2</v>
-      </c>
-      <c r="I27" s="5">
-        <v>10</v>
       </c>
     </row>
     <row r="28" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1424,10 +1439,10 @@
         <v>3.2000000000000002E-3</v>
       </c>
       <c r="H28" s="5">
+        <v>10</v>
+      </c>
+      <c r="I28" s="5">
         <v>2</v>
-      </c>
-      <c r="I28" s="5">
-        <v>10</v>
       </c>
     </row>
     <row r="29" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1453,10 +1468,10 @@
         <v>5.3E-3</v>
       </c>
       <c r="H29" s="5">
+        <v>10</v>
+      </c>
+      <c r="I29" s="5">
         <v>2</v>
-      </c>
-      <c r="I29" s="5">
-        <v>10</v>
       </c>
     </row>
     <row r="30" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1482,10 +1497,10 @@
         <v>3.5999999999999999E-3</v>
       </c>
       <c r="H30" s="5">
+        <v>10</v>
+      </c>
+      <c r="I30" s="5">
         <v>2</v>
-      </c>
-      <c r="I30" s="5">
-        <v>10</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1511,10 +1526,10 @@
         <v>4.4000000000000003E-3</v>
       </c>
       <c r="H31" s="5">
+        <v>10</v>
+      </c>
+      <c r="I31" s="5">
         <v>2</v>
-      </c>
-      <c r="I31" s="5">
-        <v>10</v>
       </c>
     </row>
     <row r="32" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1540,10 +1555,10 @@
         <v>8.5000000000000006E-3</v>
       </c>
       <c r="H32" s="5">
+        <v>10</v>
+      </c>
+      <c r="I32" s="5">
         <v>2</v>
-      </c>
-      <c r="I32" s="5">
-        <v>10</v>
       </c>
     </row>
     <row r="33" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1569,10 +1584,10 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="H33" s="5">
+        <v>10</v>
+      </c>
+      <c r="I33" s="5">
         <v>2</v>
-      </c>
-      <c r="I33" s="5">
-        <v>10</v>
       </c>
     </row>
     <row r="34" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1598,10 +1613,10 @@
         <v>6.1000000000000004E-3</v>
       </c>
       <c r="H34" s="5">
+        <v>10</v>
+      </c>
+      <c r="I34" s="5">
         <v>2</v>
-      </c>
-      <c r="I34" s="5">
-        <v>10</v>
       </c>
     </row>
     <row r="35" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1627,10 +1642,10 @@
         <v>1.0699999999999999E-2</v>
       </c>
       <c r="H35" s="5">
+        <v>10</v>
+      </c>
+      <c r="I35" s="5">
         <v>2</v>
-      </c>
-      <c r="I35" s="5">
-        <v>10</v>
       </c>
     </row>
     <row r="36" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1656,10 +1671,10 @@
         <v>7.3000000000000001E-3</v>
       </c>
       <c r="H36" s="5">
+        <v>10</v>
+      </c>
+      <c r="I36" s="5">
         <v>2</v>
-      </c>
-      <c r="I36" s="5">
-        <v>10</v>
       </c>
     </row>
     <row r="37" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1685,10 +1700,10 @@
         <v>8.2000000000000007E-3</v>
       </c>
       <c r="H37" s="5">
+        <v>10</v>
+      </c>
+      <c r="I37" s="5">
         <v>2</v>
-      </c>
-      <c r="I37" s="5">
-        <v>10</v>
       </c>
     </row>
     <row r="38" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1714,10 +1729,10 @@
         <v>6.7000000000000002E-3</v>
       </c>
       <c r="H38" s="5">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I38" s="5">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="39" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1743,10 +1758,10 @@
         <v>7.1000000000000004E-3</v>
       </c>
       <c r="H39" s="5">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I39" s="5">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="40" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1772,10 +1787,10 @@
         <v>8.0999999999999996E-3</v>
       </c>
       <c r="H40" s="5">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I40" s="5">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="41" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1801,10 +1816,10 @@
         <v>7.6E-3</v>
       </c>
       <c r="H41" s="5">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I41" s="5">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="42" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1830,10 +1845,10 @@
         <v>8.0999999999999996E-3</v>
       </c>
       <c r="H42" s="5">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I42" s="5">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="43" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1859,10 +1874,10 @@
         <v>9.5999999999999992E-3</v>
       </c>
       <c r="H43" s="5">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I43" s="5">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="44" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1888,10 +1903,10 @@
         <v>5.5999999999999999E-3</v>
       </c>
       <c r="H44" s="5">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I44" s="5">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="45" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1917,10 +1932,10 @@
         <v>6.7000000000000002E-3</v>
       </c>
       <c r="H45" s="5">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I45" s="5">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="46" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1946,10 +1961,10 @@
         <v>7.6E-3</v>
       </c>
       <c r="H46" s="5">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I46" s="5">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="47" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1975,10 +1990,10 @@
         <v>5.1999999999999998E-3</v>
       </c>
       <c r="H47" s="5">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I47" s="5">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="48" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2004,10 +2019,10 @@
         <v>7.4999999999999997E-3</v>
       </c>
       <c r="H48" s="5">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I48" s="5">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="49" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2033,10 +2048,10 @@
         <v>1.15E-2</v>
       </c>
       <c r="H49" s="5">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="I49" s="5">
-        <v>11</v>
+        <v>5</v>
       </c>
     </row>
     <row r="50" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2062,10 +2077,10 @@
         <v>8.3000000000000001E-3</v>
       </c>
       <c r="H50" s="2">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I50" s="2">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="51" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2091,10 +2106,10 @@
         <v>9.4000000000000004E-3</v>
       </c>
       <c r="H51" s="2">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I51" s="2">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="52" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2120,10 +2135,10 @@
         <v>8.5000000000000006E-3</v>
       </c>
       <c r="H52" s="2">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I52" s="2">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="53" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2149,10 +2164,10 @@
         <v>5.1999999999999998E-3</v>
       </c>
       <c r="H53" s="2">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="I53" s="2">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="54" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2178,10 +2193,10 @@
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="H54" s="2">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I54" s="2">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="55" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2207,10 +2222,10 @@
         <v>3.5000000000000001E-3</v>
       </c>
       <c r="H55" s="2">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I55" s="2">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="56" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2236,10 +2251,10 @@
         <v>6.0000000000000001E-3</v>
       </c>
       <c r="H56" s="2">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I56" s="2">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="57" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2265,10 +2280,10 @@
         <v>4.8999999999999998E-3</v>
       </c>
       <c r="H57" s="2">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I57" s="2">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="58" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2294,10 +2309,10 @@
         <v>4.7999999999999996E-3</v>
       </c>
       <c r="H58" s="2">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I58" s="2">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="59" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2323,10 +2338,10 @@
         <v>7.7999999999999996E-3</v>
       </c>
       <c r="H59" s="2">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I59" s="2">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="60" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2352,10 +2367,10 @@
         <v>9.2999999999999992E-3</v>
       </c>
       <c r="H60" s="2">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I60" s="2">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="61" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2381,10 +2396,10 @@
         <v>8.9999999999999993E-3</v>
       </c>
       <c r="H61" s="2">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I61" s="2">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="62" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2410,10 +2425,10 @@
         <v>1.1599999999999999E-2</v>
       </c>
       <c r="H62" s="2">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="I62" s="2">
-        <v>11</v>
+        <v>5</v>
       </c>
     </row>
     <row r="63" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2439,10 +2454,10 @@
         <v>1.12E-2</v>
       </c>
       <c r="H63" s="2">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I63" s="2">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="64" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2468,10 +2483,10 @@
         <v>1.11E-2</v>
       </c>
       <c r="H64" s="2">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I64" s="2">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="65" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2497,10 +2512,10 @@
         <v>1.06E-2</v>
       </c>
       <c r="H65" s="2">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I65" s="2">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="66" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2526,10 +2541,10 @@
         <v>1.3899999999999999E-2</v>
       </c>
       <c r="H66" s="2">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I66" s="2">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="67" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2555,10 +2570,10 @@
         <v>5.4999999999999997E-3</v>
       </c>
       <c r="H67" s="2">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I67" s="2">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="68" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2584,10 +2599,10 @@
         <v>5.7999999999999996E-3</v>
       </c>
       <c r="H68" s="2">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="I68" s="2">
-        <v>11</v>
+        <v>5</v>
       </c>
     </row>
     <row r="69" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2613,10 +2628,10 @@
         <v>5.4000000000000003E-3</v>
       </c>
       <c r="H69" s="2">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I69" s="2">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="70" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2642,10 +2657,10 @@
         <v>3.8999999999999998E-3</v>
       </c>
       <c r="H70" s="1">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I70" s="1">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="71" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2671,10 +2686,10 @@
         <v>5.7999999999999996E-3</v>
       </c>
       <c r="H71" s="2">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I71" s="2">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="72" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2700,10 +2715,10 @@
         <v>4.7000000000000002E-3</v>
       </c>
       <c r="H72" s="2">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I72" s="2">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="73" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2729,10 +2744,10 @@
         <v>5.4999999999999997E-3</v>
       </c>
       <c r="H73" s="2">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I73" s="2">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="74" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2758,10 +2773,10 @@
         <v>4.8999999999999998E-3</v>
       </c>
       <c r="H74" s="2">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I74" s="2">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="75" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2787,10 +2802,10 @@
         <v>4.7000000000000002E-3</v>
       </c>
       <c r="H75" s="2">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I75" s="2">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="76" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2816,10 +2831,10 @@
         <v>6.1999999999999998E-3</v>
       </c>
       <c r="H76" s="2">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I76" s="2">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="77" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2845,10 +2860,10 @@
         <v>6.1999999999999998E-3</v>
       </c>
       <c r="H77" s="2">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I77" s="2">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="78" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2874,10 +2889,10 @@
         <v>4.7999999999999996E-3</v>
       </c>
       <c r="H78" s="2">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I78" s="2">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="79" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2903,10 +2918,10 @@
         <v>3.8999999999999998E-3</v>
       </c>
       <c r="H79" s="2">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I79" s="2">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="80" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2932,13 +2947,13 @@
         <v>3.7000000000000002E-3</v>
       </c>
       <c r="H80" s="2">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I80" s="2">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="81" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="81" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
         <v>9</v>
       </c>
@@ -2961,13 +2976,13 @@
         <v>4.4000000000000003E-3</v>
       </c>
       <c r="H81" s="2">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I81" s="2">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="82" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="82" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
         <v>9</v>
       </c>
@@ -2990,13 +3005,13 @@
         <v>3.7000000000000002E-3</v>
       </c>
       <c r="H82" s="2">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I82" s="2">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="83" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="83" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
         <v>9</v>
       </c>
@@ -3019,13 +3034,13 @@
         <v>3.2000000000000002E-3</v>
       </c>
       <c r="H83" s="2">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I83" s="2">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="84" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="84" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
         <v>9</v>
       </c>
@@ -3048,13 +3063,13 @@
         <v>3.8E-3</v>
       </c>
       <c r="H84" s="2">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I84" s="2">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="85" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="85" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
         <v>9</v>
       </c>
@@ -3077,13 +3092,13 @@
         <v>4.7999999999999996E-3</v>
       </c>
       <c r="H85" s="2">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I85" s="2">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="86" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="86" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
         <v>9</v>
       </c>
@@ -3106,13 +3121,13 @@
         <v>5.7999999999999996E-3</v>
       </c>
       <c r="H86" s="2">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I86" s="2">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="87" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="87" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
         <v>9</v>
       </c>
@@ -3135,13 +3150,13 @@
         <v>6.4000000000000003E-3</v>
       </c>
       <c r="H87" s="2">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I87" s="2">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="88" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="88" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
         <v>9</v>
       </c>
@@ -3164,13 +3179,13 @@
         <v>9.7999999999999997E-3</v>
       </c>
       <c r="H88" s="2">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I88" s="2">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="89" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="89" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
         <v>9</v>
       </c>
@@ -3193,13 +3208,13 @@
         <v>8.3000000000000001E-3</v>
       </c>
       <c r="H89" s="2">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I89" s="2">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="90" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="90" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
         <v>9</v>
       </c>
@@ -3222,13 +3237,13 @@
         <v>6.8999999999999999E-3</v>
       </c>
       <c r="H90" s="2">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I90" s="2">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="91" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="91" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
         <v>9</v>
       </c>
@@ -3251,13 +3266,13 @@
         <v>6.7000000000000002E-3</v>
       </c>
       <c r="H91" s="2">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I91" s="2">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="92" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="92" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
         <v>9</v>
       </c>
@@ -3280,13 +3295,13 @@
         <v>5.1999999999999998E-3</v>
       </c>
       <c r="H92" s="2">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I92" s="2">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="93" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="93" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
         <v>9</v>
       </c>
@@ -3309,13 +3324,13 @@
         <v>6.8999999999999999E-3</v>
       </c>
       <c r="H93" s="2">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I93" s="2">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="94" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="94" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
         <v>9</v>
       </c>
@@ -3338,13 +3353,15 @@
         <v>4.5999999999999999E-3</v>
       </c>
       <c r="H94" s="2">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="I94" s="2">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="95" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="K94" s="3"/>
+      <c r="L94" s="3"/>
+    </row>
+    <row r="95" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
         <v>9</v>
       </c>
@@ -3367,13 +3384,15 @@
         <v>7.4000000000000003E-3</v>
       </c>
       <c r="H95" s="2">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I95" s="2">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="96" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="K95" s="3"/>
+      <c r="L95" s="3"/>
+    </row>
+    <row r="96" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
         <v>9</v>
       </c>
@@ -3396,13 +3415,15 @@
         <v>5.3E-3</v>
       </c>
       <c r="H96" s="2">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I96" s="2">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="97" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="K96" s="3"/>
+      <c r="L96" s="3"/>
+    </row>
+    <row r="97" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
         <v>9</v>
       </c>
@@ -3418,12 +3439,22 @@
       <c r="E97" s="5">
         <v>1</v>
       </c>
-      <c r="F97" s="2"/>
-      <c r="G97" s="2"/>
-      <c r="H97" s="2"/>
-      <c r="I97" s="2"/>
-    </row>
-    <row r="98" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F97" s="6">
+        <v>0.26290000000000002</v>
+      </c>
+      <c r="G97" s="6">
+        <v>1.26E-2</v>
+      </c>
+      <c r="H97" s="2">
+        <v>10</v>
+      </c>
+      <c r="I97" s="2">
+        <v>5</v>
+      </c>
+      <c r="K97" s="3"/>
+      <c r="L97" s="3"/>
+    </row>
+    <row r="98" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
         <v>9</v>
       </c>
@@ -3439,12 +3470,22 @@
       <c r="E98" s="5">
         <v>2</v>
       </c>
-      <c r="F98" s="2"/>
-      <c r="G98" s="2"/>
-      <c r="H98" s="2"/>
-      <c r="I98" s="2"/>
-    </row>
-    <row r="99" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F98" s="6">
+        <v>0.23119999999999999</v>
+      </c>
+      <c r="G98" s="6">
+        <v>1.1900000000000001E-2</v>
+      </c>
+      <c r="H98" s="2">
+        <v>10</v>
+      </c>
+      <c r="I98" s="2">
+        <v>5</v>
+      </c>
+      <c r="K98" s="3"/>
+      <c r="L98" s="3"/>
+    </row>
+    <row r="99" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
         <v>9</v>
       </c>
@@ -3460,12 +3501,22 @@
       <c r="E99" s="5">
         <v>3</v>
       </c>
-      <c r="F99" s="2"/>
-      <c r="G99" s="2"/>
-      <c r="H99" s="2"/>
-      <c r="I99" s="2"/>
-    </row>
-    <row r="100" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F99" s="6">
+        <v>0.4919</v>
+      </c>
+      <c r="G99" s="6">
+        <v>1.9400000000000001E-2</v>
+      </c>
+      <c r="H99" s="2">
+        <v>10</v>
+      </c>
+      <c r="I99" s="2">
+        <v>5</v>
+      </c>
+      <c r="K99" s="3"/>
+      <c r="L99" s="3"/>
+    </row>
+    <row r="100" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
         <v>9</v>
       </c>
@@ -3481,12 +3532,22 @@
       <c r="E100" s="5">
         <v>4</v>
       </c>
-      <c r="F100" s="2"/>
-      <c r="G100" s="2"/>
-      <c r="H100" s="2"/>
-      <c r="I100" s="2"/>
-    </row>
-    <row r="101" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F100" s="6">
+        <v>0.35349999999999998</v>
+      </c>
+      <c r="G100" s="6">
+        <v>1.5100000000000001E-2</v>
+      </c>
+      <c r="H100" s="2">
+        <v>10</v>
+      </c>
+      <c r="I100" s="2">
+        <v>5</v>
+      </c>
+      <c r="K100" s="3"/>
+      <c r="L100" s="3"/>
+    </row>
+    <row r="101" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
         <v>9</v>
       </c>
@@ -3502,12 +3563,22 @@
       <c r="E101" s="5">
         <v>5</v>
       </c>
-      <c r="F101" s="2"/>
-      <c r="G101" s="2"/>
-      <c r="H101" s="2"/>
-      <c r="I101" s="2"/>
-    </row>
-    <row r="102" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F101" s="6">
+        <v>0.71730000000000005</v>
+      </c>
+      <c r="G101" s="6">
+        <v>1.46E-2</v>
+      </c>
+      <c r="H101" s="2">
+        <v>10</v>
+      </c>
+      <c r="I101" s="2">
+        <v>5</v>
+      </c>
+      <c r="K101" s="3"/>
+      <c r="L101" s="3"/>
+    </row>
+    <row r="102" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="s">
         <v>9</v>
       </c>
@@ -3523,12 +3594,22 @@
       <c r="E102" s="5">
         <v>6</v>
       </c>
-      <c r="F102" s="2"/>
-      <c r="G102" s="2"/>
-      <c r="H102" s="2"/>
-      <c r="I102" s="2"/>
-    </row>
-    <row r="103" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F102" s="6">
+        <v>0.44619999999999999</v>
+      </c>
+      <c r="G102" s="6">
+        <v>1.6400000000000001E-2</v>
+      </c>
+      <c r="H102" s="2">
+        <v>10</v>
+      </c>
+      <c r="I102" s="2">
+        <v>5</v>
+      </c>
+      <c r="K102" s="3"/>
+      <c r="L102" s="3"/>
+    </row>
+    <row r="103" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="2" t="s">
         <v>9</v>
       </c>
@@ -3544,12 +3625,22 @@
       <c r="E103" s="5">
         <v>1</v>
       </c>
-      <c r="F103" s="2"/>
-      <c r="G103" s="2"/>
-      <c r="H103" s="2"/>
-      <c r="I103" s="2"/>
-    </row>
-    <row r="104" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F103" s="6">
+        <v>0.14829999999999999</v>
+      </c>
+      <c r="G103" s="2">
+        <v>1.34E-2</v>
+      </c>
+      <c r="H103" s="2">
+        <v>10</v>
+      </c>
+      <c r="I103" s="2">
+        <v>5</v>
+      </c>
+      <c r="K103" s="3"/>
+      <c r="L103" s="3"/>
+    </row>
+    <row r="104" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="2" t="s">
         <v>9</v>
       </c>
@@ -3562,15 +3653,16 @@
       <c r="D104" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E104" s="5">
-        <v>2</v>
-      </c>
-      <c r="F104" s="2"/>
-      <c r="G104" s="2"/>
-      <c r="H104" s="2"/>
-      <c r="I104" s="2"/>
-    </row>
-    <row r="105" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E104" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="F104" s="6">
+        <v>0.1187</v>
+      </c>
+      <c r="K104" s="3"/>
+      <c r="L104" s="3"/>
+    </row>
+    <row r="105" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" s="2" t="s">
         <v>9</v>
       </c>
@@ -3583,15 +3675,25 @@
       <c r="D105" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E105" s="5">
-        <v>3</v>
-      </c>
-      <c r="F105" s="2"/>
-      <c r="G105" s="2"/>
-      <c r="H105" s="2"/>
-      <c r="I105" s="2"/>
-    </row>
-    <row r="106" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E105" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="F105" s="6">
+        <v>8.3099999999999993E-2</v>
+      </c>
+      <c r="G105" s="2">
+        <v>1.6000000000000001E-3</v>
+      </c>
+      <c r="H105" s="2">
+        <v>1</v>
+      </c>
+      <c r="I105" s="2">
+        <v>2002</v>
+      </c>
+      <c r="K105" s="3"/>
+      <c r="L105" s="3"/>
+    </row>
+    <row r="106" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="2" t="s">
         <v>9</v>
       </c>
@@ -3605,14 +3707,22 @@
         <v>11</v>
       </c>
       <c r="E106" s="5">
-        <v>4</v>
-      </c>
-      <c r="F106" s="2"/>
-      <c r="G106" s="2"/>
-      <c r="H106" s="2"/>
-      <c r="I106" s="2"/>
-    </row>
-    <row r="107" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="F106" s="6">
+        <v>0.24970000000000001</v>
+      </c>
+      <c r="G106" s="2">
+        <v>9.7999999999999997E-3</v>
+      </c>
+      <c r="H106" s="2">
+        <v>10</v>
+      </c>
+      <c r="I106" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="107" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" s="2" t="s">
         <v>9</v>
       </c>
@@ -3626,14 +3736,22 @@
         <v>11</v>
       </c>
       <c r="E107" s="5">
-        <v>5</v>
-      </c>
-      <c r="F107" s="2"/>
-      <c r="G107" s="2"/>
-      <c r="H107" s="2"/>
-      <c r="I107" s="2"/>
-    </row>
-    <row r="108" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="F107" s="6">
+        <v>0.15529999999999999</v>
+      </c>
+      <c r="G107" s="2">
+        <v>8.3000000000000001E-3</v>
+      </c>
+      <c r="H107" s="2">
+        <v>10</v>
+      </c>
+      <c r="I107" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="108" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" s="2" t="s">
         <v>9</v>
       </c>
@@ -3647,14 +3765,22 @@
         <v>11</v>
       </c>
       <c r="E108" s="5">
-        <v>6</v>
-      </c>
-      <c r="F108" s="2"/>
-      <c r="G108" s="2"/>
-      <c r="H108" s="2"/>
-      <c r="I108" s="2"/>
-    </row>
-    <row r="109" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="F108" s="6">
+        <v>0.15279999999999999</v>
+      </c>
+      <c r="G108" s="2">
+        <v>3.2800000000000003E-2</v>
+      </c>
+      <c r="H108" s="2">
+        <v>10</v>
+      </c>
+      <c r="I108" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="109" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" s="2" t="s">
         <v>9</v>
       </c>
@@ -3668,14 +3794,22 @@
         <v>11</v>
       </c>
       <c r="E109" s="5">
-        <v>10</v>
-      </c>
-      <c r="F109" s="2"/>
-      <c r="G109" s="2"/>
-      <c r="H109" s="2"/>
-      <c r="I109" s="2"/>
-    </row>
-    <row r="110" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="F109" s="6">
+        <v>0.113</v>
+      </c>
+      <c r="G109" s="2">
+        <v>2.24E-2</v>
+      </c>
+      <c r="H109" s="2">
+        <v>10</v>
+      </c>
+      <c r="I109" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="110" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" s="2" t="s">
         <v>9</v>
       </c>
@@ -3691,12 +3825,20 @@
       <c r="E110" s="5">
         <v>1</v>
       </c>
-      <c r="F110" s="2"/>
-      <c r="G110" s="2"/>
-      <c r="H110" s="2"/>
-      <c r="I110" s="2"/>
-    </row>
-    <row r="111" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F110" s="2">
+        <v>0.31559999999999999</v>
+      </c>
+      <c r="G110" s="2">
+        <v>1.95E-2</v>
+      </c>
+      <c r="H110" s="2">
+        <v>10</v>
+      </c>
+      <c r="I110" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="111" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" s="2" t="s">
         <v>9</v>
       </c>
@@ -3712,12 +3854,20 @@
       <c r="E111" s="5">
         <v>2</v>
       </c>
-      <c r="F111" s="2"/>
-      <c r="G111" s="2"/>
-      <c r="H111" s="2"/>
-      <c r="I111" s="2"/>
-    </row>
-    <row r="112" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F111" s="2">
+        <v>0.27150000000000002</v>
+      </c>
+      <c r="G111" s="2">
+        <v>1.7600000000000001E-2</v>
+      </c>
+      <c r="H111" s="2">
+        <v>10</v>
+      </c>
+      <c r="I111" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="112" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" s="2" t="s">
         <v>9</v>
       </c>
@@ -3733,10 +3883,18 @@
       <c r="E112" s="5">
         <v>3</v>
       </c>
-      <c r="F112" s="2"/>
-      <c r="G112" s="2"/>
-      <c r="H112" s="2"/>
-      <c r="I112" s="2"/>
+      <c r="F112" s="2">
+        <v>0.38640000000000002</v>
+      </c>
+      <c r="G112" s="2">
+        <v>2.5899999999999999E-2</v>
+      </c>
+      <c r="H112" s="2">
+        <v>10</v>
+      </c>
+      <c r="I112" s="2">
+        <v>5</v>
+      </c>
     </row>
     <row r="113" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" s="2" t="s">
@@ -3754,10 +3912,18 @@
       <c r="E113" s="5">
         <v>4</v>
       </c>
-      <c r="F113" s="2"/>
-      <c r="G113" s="2"/>
-      <c r="H113" s="2"/>
-      <c r="I113" s="2"/>
+      <c r="F113" s="2">
+        <v>0.32319999999999999</v>
+      </c>
+      <c r="G113" s="2">
+        <v>1.41E-2</v>
+      </c>
+      <c r="H113" s="2">
+        <v>10</v>
+      </c>
+      <c r="I113" s="2">
+        <v>5</v>
+      </c>
     </row>
     <row r="114" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114" s="2" t="s">
@@ -3775,10 +3941,18 @@
       <c r="E114" s="5">
         <v>5</v>
       </c>
-      <c r="F114" s="2"/>
-      <c r="G114" s="2"/>
-      <c r="H114" s="2"/>
-      <c r="I114" s="2"/>
+      <c r="F114" s="2">
+        <v>0.312</v>
+      </c>
+      <c r="G114" s="2">
+        <v>1.89E-2</v>
+      </c>
+      <c r="H114" s="2">
+        <v>10</v>
+      </c>
+      <c r="I114" s="2">
+        <v>5</v>
+      </c>
     </row>
     <row r="115" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" s="2" t="s">
@@ -3796,10 +3970,18 @@
       <c r="E115" s="5">
         <v>6</v>
       </c>
-      <c r="F115" s="2"/>
-      <c r="G115" s="2"/>
-      <c r="H115" s="2"/>
-      <c r="I115" s="2"/>
+      <c r="F115" s="2">
+        <v>0.33129999999999998</v>
+      </c>
+      <c r="G115" s="2">
+        <v>2.0299999999999999E-2</v>
+      </c>
+      <c r="H115" s="2">
+        <v>10</v>
+      </c>
+      <c r="I115" s="2">
+        <v>5</v>
+      </c>
     </row>
     <row r="116" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116" s="2" t="s">
@@ -3817,10 +3999,18 @@
       <c r="E116" s="5">
         <v>1</v>
       </c>
-      <c r="F116" s="2"/>
-      <c r="G116" s="2"/>
-      <c r="H116" s="2"/>
-      <c r="I116" s="2"/>
+      <c r="F116" s="2">
+        <v>0.24790000000000001</v>
+      </c>
+      <c r="G116" s="2">
+        <v>1.6999999999999999E-3</v>
+      </c>
+      <c r="H116" s="2">
+        <v>10</v>
+      </c>
+      <c r="I116" s="2">
+        <v>5</v>
+      </c>
     </row>
     <row r="117" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A117" s="2" t="s">
@@ -3838,10 +4028,18 @@
       <c r="E117" s="5">
         <v>2</v>
       </c>
-      <c r="F117" s="2"/>
-      <c r="G117" s="2"/>
-      <c r="H117" s="2"/>
-      <c r="I117" s="2"/>
+      <c r="F117" s="2">
+        <v>0.18890000000000001</v>
+      </c>
+      <c r="G117" s="2">
+        <v>2.3999999999999998E-3</v>
+      </c>
+      <c r="H117" s="2">
+        <v>10</v>
+      </c>
+      <c r="I117" s="2">
+        <v>5</v>
+      </c>
     </row>
     <row r="118" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118" s="2" t="s">
@@ -3859,10 +4057,18 @@
       <c r="E118" s="5">
         <v>3</v>
       </c>
-      <c r="F118" s="2"/>
-      <c r="G118" s="2"/>
-      <c r="H118" s="2"/>
-      <c r="I118" s="2"/>
+      <c r="F118" s="2">
+        <v>0.23039999999999999</v>
+      </c>
+      <c r="G118" s="2">
+        <v>2.3E-3</v>
+      </c>
+      <c r="H118" s="2">
+        <v>10</v>
+      </c>
+      <c r="I118" s="2">
+        <v>5</v>
+      </c>
     </row>
     <row r="119" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A119" s="2" t="s">
@@ -3880,10 +4086,18 @@
       <c r="E119" s="5">
         <v>4</v>
       </c>
-      <c r="F119" s="2"/>
-      <c r="G119" s="2"/>
-      <c r="H119" s="2"/>
-      <c r="I119" s="2"/>
+      <c r="F119" s="2">
+        <v>0.13389999999999999</v>
+      </c>
+      <c r="G119" s="2">
+        <v>1.2999999999999999E-3</v>
+      </c>
+      <c r="H119" s="2">
+        <v>10</v>
+      </c>
+      <c r="I119" s="2">
+        <v>5</v>
+      </c>
     </row>
     <row r="120" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A120" s="2" t="s">
@@ -3902,9 +4116,15 @@
         <v>5</v>
       </c>
       <c r="F120" s="2"/>
-      <c r="G120" s="2"/>
-      <c r="H120" s="2"/>
-      <c r="I120" s="2"/>
+      <c r="G120" s="2">
+        <v>1.6000000000000001E-3</v>
+      </c>
+      <c r="H120" s="2">
+        <v>10</v>
+      </c>
+      <c r="I120" s="2">
+        <v>5</v>
+      </c>
     </row>
     <row r="121" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A121" s="2" t="s">
@@ -3922,10 +4142,18 @@
       <c r="E121" s="5">
         <v>1</v>
       </c>
-      <c r="F121" s="2"/>
-      <c r="G121" s="2"/>
-      <c r="H121" s="2"/>
-      <c r="I121" s="2"/>
+      <c r="F121" s="2">
+        <v>0.1593</v>
+      </c>
+      <c r="G121" s="2">
+        <v>2.4E-2</v>
+      </c>
+      <c r="H121" s="2">
+        <v>10</v>
+      </c>
+      <c r="I121" s="2">
+        <v>5</v>
+      </c>
     </row>
     <row r="122" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A122" s="2" t="s">
@@ -3943,10 +4171,18 @@
       <c r="E122" s="5">
         <v>3</v>
       </c>
-      <c r="F122" s="2"/>
-      <c r="G122" s="2"/>
-      <c r="H122" s="2"/>
-      <c r="I122" s="2"/>
+      <c r="F122" s="2">
+        <v>0.20949999999999999</v>
+      </c>
+      <c r="G122" s="2">
+        <v>1.06E-2</v>
+      </c>
+      <c r="H122" s="2">
+        <v>10</v>
+      </c>
+      <c r="I122" s="2">
+        <v>5</v>
+      </c>
     </row>
     <row r="123" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A123" s="2" t="s">
@@ -3964,10 +4200,18 @@
       <c r="E123" s="5">
         <v>5</v>
       </c>
-      <c r="F123" s="2"/>
-      <c r="G123" s="2"/>
-      <c r="H123" s="2"/>
-      <c r="I123" s="2"/>
+      <c r="F123" s="2">
+        <v>0.1757</v>
+      </c>
+      <c r="G123" s="2">
+        <v>1.3299999999999999E-2</v>
+      </c>
+      <c r="H123" s="2">
+        <v>10</v>
+      </c>
+      <c r="I123" s="2">
+        <v>5</v>
+      </c>
     </row>
     <row r="124" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A124" s="2" t="s">
@@ -3985,10 +4229,18 @@
       <c r="E124" s="5">
         <v>6</v>
       </c>
-      <c r="F124" s="2"/>
-      <c r="G124" s="2"/>
-      <c r="H124" s="2"/>
-      <c r="I124" s="2"/>
+      <c r="F124" s="2">
+        <v>7.9299999999999995E-2</v>
+      </c>
+      <c r="G124" s="2">
+        <v>2.4500000000000001E-2</v>
+      </c>
+      <c r="H124" s="2">
+        <v>10</v>
+      </c>
+      <c r="I124" s="2">
+        <v>5</v>
+      </c>
     </row>
     <row r="125" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A125" s="2" t="s">
@@ -4006,10 +4258,18 @@
       <c r="E125" s="5">
         <v>7</v>
       </c>
-      <c r="F125" s="2"/>
-      <c r="G125" s="2"/>
-      <c r="H125" s="2"/>
-      <c r="I125" s="2"/>
+      <c r="F125" s="2">
+        <v>0.1114</v>
+      </c>
+      <c r="G125" s="2">
+        <v>1.4500000000000001E-2</v>
+      </c>
+      <c r="H125" s="2">
+        <v>10</v>
+      </c>
+      <c r="I125" s="2">
+        <v>5</v>
+      </c>
     </row>
     <row r="126" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A126" s="2" t="s">
@@ -4027,10 +4287,16 @@
       <c r="E126" s="5">
         <v>8</v>
       </c>
-      <c r="F126" s="2"/>
+      <c r="F126" s="2">
+        <v>0.1202</v>
+      </c>
       <c r="G126" s="2"/>
-      <c r="H126" s="2"/>
-      <c r="I126" s="2"/>
+      <c r="H126" s="2">
+        <v>10</v>
+      </c>
+      <c r="I126" s="2">
+        <v>5</v>
+      </c>
     </row>
     <row r="127" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A127" s="2" t="s">
@@ -4048,10 +4314,18 @@
       <c r="E127" s="5">
         <v>1</v>
       </c>
-      <c r="F127" s="2"/>
-      <c r="G127" s="2"/>
-      <c r="H127" s="2"/>
-      <c r="I127" s="2"/>
+      <c r="F127" s="2">
+        <v>0.16089999999999999</v>
+      </c>
+      <c r="G127" s="2">
+        <v>1.0200000000000001E-2</v>
+      </c>
+      <c r="H127" s="2">
+        <v>10</v>
+      </c>
+      <c r="I127" s="2">
+        <v>5</v>
+      </c>
     </row>
     <row r="128" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A128" s="2" t="s">
@@ -4069,10 +4343,18 @@
       <c r="E128" s="5">
         <v>2</v>
       </c>
-      <c r="F128" s="2"/>
-      <c r="G128" s="2"/>
-      <c r="H128" s="2"/>
-      <c r="I128" s="2"/>
+      <c r="F128" s="2">
+        <v>0.15570000000000001</v>
+      </c>
+      <c r="G128" s="2">
+        <v>7.7000000000000002E-3</v>
+      </c>
+      <c r="H128" s="2">
+        <v>10</v>
+      </c>
+      <c r="I128" s="2">
+        <v>5</v>
+      </c>
     </row>
     <row r="129" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A129" s="2" t="s">
@@ -4090,10 +4372,18 @@
       <c r="E129" s="5">
         <v>3</v>
       </c>
-      <c r="F129" s="2"/>
-      <c r="G129" s="2"/>
-      <c r="H129" s="2"/>
-      <c r="I129" s="2"/>
+      <c r="F129" s="2">
+        <v>0.10829999999999999</v>
+      </c>
+      <c r="G129" s="2">
+        <v>5.1000000000000004E-3</v>
+      </c>
+      <c r="H129" s="2">
+        <v>10</v>
+      </c>
+      <c r="I129" s="2">
+        <v>5</v>
+      </c>
     </row>
     <row r="130" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A130" s="2" t="s">
@@ -4111,10 +4401,18 @@
       <c r="E130" s="5">
         <v>4</v>
       </c>
-      <c r="F130" s="2"/>
-      <c r="G130" s="2"/>
-      <c r="H130" s="2"/>
-      <c r="I130" s="2"/>
+      <c r="F130" s="2">
+        <v>0.1234</v>
+      </c>
+      <c r="G130" s="2">
+        <v>6.7000000000000002E-3</v>
+      </c>
+      <c r="H130" s="2">
+        <v>10</v>
+      </c>
+      <c r="I130" s="2">
+        <v>5</v>
+      </c>
     </row>
     <row r="131" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A131" s="2" t="s">
@@ -4132,10 +4430,18 @@
       <c r="E131" s="5">
         <v>5</v>
       </c>
-      <c r="F131" s="2"/>
-      <c r="G131" s="2"/>
-      <c r="H131" s="2"/>
-      <c r="I131" s="2"/>
+      <c r="F131" s="2">
+        <v>0.16200000000000001</v>
+      </c>
+      <c r="G131" s="2">
+        <v>9.5999999999999992E-3</v>
+      </c>
+      <c r="H131" s="2">
+        <v>10</v>
+      </c>
+      <c r="I131" s="2">
+        <v>5</v>
+      </c>
     </row>
     <row r="132" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A132" s="2" t="s">
@@ -4153,10 +4459,18 @@
       <c r="E132" s="5">
         <v>6</v>
       </c>
-      <c r="F132" s="2"/>
-      <c r="G132" s="2"/>
-      <c r="H132" s="2"/>
-      <c r="I132" s="2"/>
+      <c r="F132" s="2">
+        <v>0.2112</v>
+      </c>
+      <c r="G132" s="2">
+        <v>1.37E-2</v>
+      </c>
+      <c r="H132" s="2">
+        <v>10</v>
+      </c>
+      <c r="I132" s="2">
+        <v>5</v>
+      </c>
     </row>
     <row r="133" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A133" s="2" t="s">
@@ -4174,10 +4488,18 @@
       <c r="E133" s="5">
         <v>1</v>
       </c>
-      <c r="F133" s="2"/>
-      <c r="G133" s="2"/>
-      <c r="H133" s="2"/>
-      <c r="I133" s="2"/>
+      <c r="F133" s="2">
+        <v>0.14749999999999999</v>
+      </c>
+      <c r="G133" s="2">
+        <v>9.5999999999999992E-3</v>
+      </c>
+      <c r="H133" s="2">
+        <v>10</v>
+      </c>
+      <c r="I133" s="2">
+        <v>5</v>
+      </c>
     </row>
     <row r="134" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A134" s="2" t="s">
@@ -4195,10 +4517,18 @@
       <c r="E134" s="5">
         <v>2</v>
       </c>
-      <c r="F134" s="2"/>
-      <c r="G134" s="2"/>
-      <c r="H134" s="2"/>
-      <c r="I134" s="2"/>
+      <c r="F134" s="2">
+        <v>0.1658</v>
+      </c>
+      <c r="G134" s="2">
+        <v>9.7999999999999997E-3</v>
+      </c>
+      <c r="H134" s="2">
+        <v>10</v>
+      </c>
+      <c r="I134" s="2">
+        <v>5</v>
+      </c>
     </row>
     <row r="135" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A135" s="2" t="s">
@@ -4216,10 +4546,18 @@
       <c r="E135" s="5">
         <v>3</v>
       </c>
-      <c r="F135" s="2"/>
-      <c r="G135" s="2"/>
-      <c r="H135" s="2"/>
-      <c r="I135" s="2"/>
+      <c r="F135" s="2">
+        <v>0.1177</v>
+      </c>
+      <c r="G135" s="2">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="H135" s="2">
+        <v>10</v>
+      </c>
+      <c r="I135" s="2">
+        <v>5</v>
+      </c>
     </row>
     <row r="136" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A136" s="2" t="s">
@@ -4237,10 +4575,18 @@
       <c r="E136" s="5">
         <v>4</v>
       </c>
-      <c r="F136" s="2"/>
-      <c r="G136" s="2"/>
-      <c r="H136" s="2"/>
-      <c r="I136" s="2"/>
+      <c r="F136" s="2">
+        <v>0.217</v>
+      </c>
+      <c r="G136" s="2">
+        <v>1.0699999999999999E-2</v>
+      </c>
+      <c r="H136" s="2">
+        <v>10</v>
+      </c>
+      <c r="I136" s="2">
+        <v>5</v>
+      </c>
     </row>
     <row r="137" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A137" s="2" t="s">
@@ -4258,10 +4604,18 @@
       <c r="E137" s="5">
         <v>5</v>
       </c>
-      <c r="F137" s="2"/>
-      <c r="G137" s="2"/>
-      <c r="H137" s="2"/>
-      <c r="I137" s="2"/>
+      <c r="F137" s="2">
+        <v>0.1386</v>
+      </c>
+      <c r="G137" s="2">
+        <v>5.7000000000000002E-3</v>
+      </c>
+      <c r="H137" s="2">
+        <v>10</v>
+      </c>
+      <c r="I137" s="2">
+        <v>5</v>
+      </c>
     </row>
     <row r="138" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A138" s="2" t="s">
@@ -4279,12 +4633,20 @@
       <c r="E138" s="5">
         <v>6</v>
       </c>
-      <c r="F138" s="2"/>
-      <c r="G138" s="2"/>
-      <c r="H138" s="2"/>
-      <c r="I138" s="2"/>
-    </row>
-    <row r="139" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F138" s="2">
+        <v>0.1208</v>
+      </c>
+      <c r="G138" s="2">
+        <v>7.4000000000000003E-3</v>
+      </c>
+      <c r="H138" s="2">
+        <v>10</v>
+      </c>
+      <c r="I138" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="139" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A139" s="2" t="s">
         <v>9</v>
       </c>
@@ -4300,10 +4662,18 @@
       <c r="E139" s="5">
         <v>1</v>
       </c>
-      <c r="F139" s="2"/>
-      <c r="G139" s="2"/>
-      <c r="H139" s="2"/>
-      <c r="I139" s="2"/>
+      <c r="F139" s="2">
+        <v>0.1244</v>
+      </c>
+      <c r="G139" s="2">
+        <v>4.4000000000000003E-3</v>
+      </c>
+      <c r="H139" s="2">
+        <v>10</v>
+      </c>
+      <c r="I139" s="2">
+        <v>5</v>
+      </c>
     </row>
     <row r="140" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A140" s="2" t="s">
@@ -4321,10 +4691,18 @@
       <c r="E140" s="5">
         <v>2</v>
       </c>
-      <c r="F140" s="2"/>
-      <c r="G140" s="2"/>
-      <c r="H140" s="2"/>
-      <c r="I140" s="2"/>
+      <c r="F140" s="2">
+        <v>0.20930000000000001</v>
+      </c>
+      <c r="G140" s="2">
+        <v>5.7000000000000002E-3</v>
+      </c>
+      <c r="H140" s="2">
+        <v>10</v>
+      </c>
+      <c r="I140" s="2">
+        <v>5</v>
+      </c>
     </row>
     <row r="141" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A141" s="2" t="s">
@@ -4342,10 +4720,18 @@
       <c r="E141" s="5">
         <v>3</v>
       </c>
-      <c r="F141" s="2"/>
-      <c r="G141" s="2"/>
-      <c r="H141" s="2"/>
-      <c r="I141" s="2"/>
+      <c r="F141" s="2">
+        <v>0.1358</v>
+      </c>
+      <c r="G141" s="2">
+        <v>4.7999999999999996E-3</v>
+      </c>
+      <c r="H141" s="2">
+        <v>10</v>
+      </c>
+      <c r="I141" s="2">
+        <v>5</v>
+      </c>
     </row>
     <row r="142" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A142" s="2" t="s">
@@ -4363,10 +4749,18 @@
       <c r="E142" s="5">
         <v>4</v>
       </c>
-      <c r="F142" s="2"/>
-      <c r="G142" s="2"/>
-      <c r="H142" s="2"/>
-      <c r="I142" s="2"/>
+      <c r="F142" s="2">
+        <v>6.6900000000000001E-2</v>
+      </c>
+      <c r="G142" s="2">
+        <v>5.7000000000000002E-3</v>
+      </c>
+      <c r="H142" s="2">
+        <v>10</v>
+      </c>
+      <c r="I142" s="2">
+        <v>5</v>
+      </c>
     </row>
     <row r="143" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A143" s="2" t="s">
@@ -4384,10 +4778,18 @@
       <c r="E143" s="5">
         <v>5</v>
       </c>
-      <c r="F143" s="2"/>
-      <c r="G143" s="2"/>
-      <c r="H143" s="2"/>
-      <c r="I143" s="2"/>
+      <c r="F143" s="2">
+        <v>8.0100000000000005E-2</v>
+      </c>
+      <c r="G143" s="2">
+        <v>4.5999999999999999E-3</v>
+      </c>
+      <c r="H143" s="2">
+        <v>10</v>
+      </c>
+      <c r="I143" s="2">
+        <v>5</v>
+      </c>
     </row>
     <row r="144" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A144" s="2" t="s">
@@ -4405,10 +4807,18 @@
       <c r="E144" s="5">
         <v>6</v>
       </c>
-      <c r="F144" s="2"/>
-      <c r="G144" s="2"/>
-      <c r="H144" s="2"/>
-      <c r="I144" s="2"/>
+      <c r="F144" s="2">
+        <v>7.3700000000000002E-2</v>
+      </c>
+      <c r="G144" s="2">
+        <v>4.8999999999999998E-3</v>
+      </c>
+      <c r="H144" s="2">
+        <v>10</v>
+      </c>
+      <c r="I144" s="2">
+        <v>5</v>
+      </c>
     </row>
     <row r="145" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A145" s="2" t="s">
@@ -4426,10 +4836,18 @@
       <c r="E145" s="5">
         <v>1</v>
       </c>
-      <c r="F145" s="2"/>
-      <c r="G145" s="2"/>
-      <c r="H145" s="2"/>
-      <c r="I145" s="2"/>
+      <c r="F145" s="2">
+        <v>9.4799999999999995E-2</v>
+      </c>
+      <c r="G145" s="2">
+        <v>5.5999999999999999E-3</v>
+      </c>
+      <c r="H145" s="2">
+        <v>10</v>
+      </c>
+      <c r="I145" s="2">
+        <v>5</v>
+      </c>
     </row>
     <row r="146" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A146" s="2" t="s">
@@ -4447,10 +4865,18 @@
       <c r="E146" s="5">
         <v>2</v>
       </c>
-      <c r="F146" s="2"/>
-      <c r="G146" s="2"/>
-      <c r="H146" s="2"/>
-      <c r="I146" s="2"/>
+      <c r="F146" s="2">
+        <v>8.0199999999999994E-2</v>
+      </c>
+      <c r="G146" s="2">
+        <v>4.7999999999999996E-3</v>
+      </c>
+      <c r="H146" s="2">
+        <v>10</v>
+      </c>
+      <c r="I146" s="2">
+        <v>5</v>
+      </c>
     </row>
     <row r="147" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A147" s="2" t="s">
@@ -4468,10 +4894,18 @@
       <c r="E147" s="5">
         <v>3</v>
       </c>
-      <c r="F147" s="2"/>
-      <c r="G147" s="2"/>
-      <c r="H147" s="2"/>
-      <c r="I147" s="2"/>
+      <c r="F147" s="2">
+        <v>5.21E-2</v>
+      </c>
+      <c r="G147" s="2">
+        <v>5.1000000000000004E-3</v>
+      </c>
+      <c r="H147" s="2">
+        <v>10</v>
+      </c>
+      <c r="I147" s="2">
+        <v>5</v>
+      </c>
     </row>
     <row r="148" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A148" s="2" t="s">
@@ -4489,10 +4923,18 @@
       <c r="E148" s="5">
         <v>6</v>
       </c>
-      <c r="F148" s="2"/>
-      <c r="G148" s="2"/>
-      <c r="H148" s="2"/>
-      <c r="I148" s="2"/>
+      <c r="F148" s="2">
+        <v>0.1079</v>
+      </c>
+      <c r="G148" s="2">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="H148" s="2">
+        <v>9</v>
+      </c>
+      <c r="I148" s="2">
+        <v>5</v>
+      </c>
     </row>
     <row r="149" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A149" s="2" t="s">
@@ -4510,10 +4952,18 @@
       <c r="E149" s="5">
         <v>8</v>
       </c>
-      <c r="F149" s="2"/>
-      <c r="G149" s="2"/>
-      <c r="H149" s="2"/>
-      <c r="I149" s="2"/>
+      <c r="F149" s="2">
+        <v>0.13900000000000001</v>
+      </c>
+      <c r="G149" s="2">
+        <v>3.5999999999999999E-3</v>
+      </c>
+      <c r="H149" s="2">
+        <v>9</v>
+      </c>
+      <c r="I149" s="2">
+        <v>5</v>
+      </c>
     </row>
     <row r="150" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A150" s="2" t="s">
@@ -4531,10 +4981,18 @@
       <c r="E150" s="5">
         <v>9</v>
       </c>
-      <c r="F150" s="2"/>
-      <c r="G150" s="2"/>
-      <c r="H150" s="2"/>
-      <c r="I150" s="2"/>
+      <c r="F150" s="2">
+        <v>0.1225</v>
+      </c>
+      <c r="G150" s="2">
+        <v>4.1000000000000003E-3</v>
+      </c>
+      <c r="H150" s="3">
+        <v>10</v>
+      </c>
+      <c r="I150" s="3">
+        <v>5</v>
+      </c>
     </row>
     <row r="151" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A151" s="2" t="s">
@@ -4559,10 +5017,10 @@
         <v>6.1999999999999998E-3</v>
       </c>
       <c r="H151" s="3">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I151" s="3">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="152" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -4588,10 +5046,10 @@
         <v>7.9000000000000008E-3</v>
       </c>
       <c r="H152" s="3">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I152" s="3">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="153" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -4617,10 +5075,10 @@
         <v>6.8999999999999999E-3</v>
       </c>
       <c r="H153" s="3">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I153" s="3">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="154" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -4646,10 +5104,10 @@
         <v>7.7999999999999996E-3</v>
       </c>
       <c r="H154" s="3">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I154" s="3">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="155" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -4675,10 +5133,10 @@
         <v>6.3E-3</v>
       </c>
       <c r="H155" s="3">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I155" s="3">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="156" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -4704,38 +5162,14 @@
         <v>6.3E-3</v>
       </c>
       <c r="H156" s="3">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I156" s="3">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>